<commit_message>
TODO sortLineas in mutations
</commit_message>
<xml_diff>
--- a/topdown.xlsx
+++ b/topdown.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.arashiro\proyectos\Code\syllabus5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="80" windowWidth="18900" windowHeight="7340" activeTab="3"/>
+    <workbookView xWindow="165" yWindow="75" windowWidth="18900" windowHeight="7335" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">datos!$A$1:$F$65</definedName>
     <definedName name="_xlnm.Extract" localSheetId="1">campos!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -621,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -665,6 +670,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -685,6 +693,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -733,7 +744,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -768,7 +779,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -983,13 +994,13 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -997,177 +1008,177 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>18</v>
       </c>
@@ -1186,27 +1197,27 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1256,7 +1267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1282,7 +1293,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>+A3</f>
         <v>generales</v>
@@ -1319,14 +1330,14 @@
       <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1334,7 +1345,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -1345,7 +1356,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>36</v>
       </c>
@@ -1356,7 +1367,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>37</v>
       </c>
@@ -1367,7 +1378,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -1378,7 +1389,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>39</v>
       </c>
@@ -1389,7 +1400,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>40</v>
       </c>
@@ -1400,7 +1411,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1408,12 +1419,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1421,32 +1432,32 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1454,32 +1465,32 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -1487,12 +1498,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -1506,60 +1517,60 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="18" t="s">
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="16" t="s">
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+    </row>
+    <row r="36" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="19" t="s">
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="16" t="s">
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="38" spans="1:10" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="16" t="s">
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1567,24 +1578,24 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="16" t="s">
+    <row r="40" spans="1:10" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16" t="s">
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="19" t="s">
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3</v>
       </c>
@@ -1596,113 +1607,113 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="16" t="s">
+    <row r="42" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16" t="s">
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16" t="s">
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16"/>
-    </row>
-    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="16" t="s">
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
       <c r="H43" t="s">
         <v>78</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4</v>
       </c>
       <c r="B44" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
       <c r="H44" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>80</v>
       </c>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
       <c r="H45" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>81</v>
       </c>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
       <c r="H46" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>83</v>
       </c>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B50" s="17" t="s">
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5</v>
       </c>
@@ -1721,7 +1732,7 @@
       </c>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>88</v>
       </c>
@@ -1732,7 +1743,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
@@ -1742,7 +1753,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
@@ -1752,7 +1763,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
@@ -1762,7 +1773,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
@@ -1772,7 +1783,7 @@
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -1782,7 +1793,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
@@ -1792,7 +1803,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
@@ -1802,7 +1813,7 @@
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>90</v>
       </c>
@@ -1810,37 +1821,37 @@
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>98</v>
       </c>
@@ -1848,38 +1859,38 @@
         <v>99</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>101</v>
       </c>
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>106</v>
       </c>
@@ -1887,7 +1898,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1</v>
       </c>
@@ -1895,22 +1906,22 @@
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2</v>
       </c>
@@ -1918,22 +1929,22 @@
         <v>133</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>3</v>
       </c>
@@ -1941,17 +1952,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>118</v>
       </c>
@@ -1980,29 +1991,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L65"/>
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.453125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.1796875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="9" style="7" customWidth="1"/>
     <col min="8" max="8" width="9" style="14" customWidth="1"/>
     <col min="9" max="9" width="9" style="12" customWidth="1"/>
-    <col min="10" max="10" width="28.1796875" style="7" customWidth="1"/>
-    <col min="11" max="11" width="10.90625" style="2"/>
-    <col min="12" max="12" width="10.90625" style="10"/>
+    <col min="10" max="10" width="28.140625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="2"/>
+    <col min="12" max="12" width="10.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -2031,7 +2042,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>152</v>
       </c>
@@ -2058,19 +2069,19 @@
         <v>11</v>
       </c>
       <c r="J2" s="7" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H2&amp;", '"&amp;I$1&amp;"': '"&amp;I2&amp;"', '"&amp;C$1&amp;"': "&amp;C2&amp;", '"&amp;D$1&amp;"': "&amp;D2&amp;", '"&amp;E$1&amp;"': '"&amp;E2&amp;"', '"&amp;F$1&amp;"': '"&amp;F2&amp;"', '"&amp;G$1&amp;"':"&amp;G2&amp;"}, "</f>
+        <f t="shared" ref="J2:J33" si="1">+"{ '"&amp;H$1&amp;"': "&amp;H2&amp;", '"&amp;I$1&amp;"': '"&amp;I2&amp;"', '"&amp;C$1&amp;"': "&amp;C2&amp;", '"&amp;D$1&amp;"': "&amp;D2&amp;", '"&amp;E$1&amp;"': '"&amp;E2&amp;"', '"&amp;F$1&amp;"': '"&amp;F2&amp;"', '"&amp;G$1&amp;"':"&amp;G2&amp;"}, "</f>
         <v xml:space="preserve">{ 'reg': 11, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'center', 'texto': 'CONTABILIDAD GERENCIAL', 'offset':1}, </v>
       </c>
       <c r="K2" s="2" t="str">
-        <f>IF(B1=B2,CONCATENATE(K1,J2),J2)</f>
+        <f t="shared" ref="K2:K33" si="2">IF(B1=B2,CONCATENATE(K1,J2),J2)</f>
         <v xml:space="preserve">{ 'reg': 11, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'center', 'texto': 'CONTABILIDAD GERENCIAL', 'offset':1}, </v>
       </c>
       <c r="L2" s="11" t="str">
-        <f>IF(B2=B3,"","{'"&amp;B$1&amp;"': "&amp;B2&amp;", 'editing': false, 'tipo': '"&amp;A2&amp;"', 'data': "&amp;"["&amp;K2&amp;"],  },")</f>
+        <f t="shared" ref="L2:L33" si="3">IF(B2=B3,"","{'"&amp;B$1&amp;"': "&amp;B2&amp;", 'editing': false, 'tipo': '"&amp;A2&amp;"', 'data': "&amp;"["&amp;K2&amp;"],  },")</f>
         <v>{'row': 1, 'editing': false, 'tipo': 'titulo0', 'data': [{ 'reg': 11, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'center', 'texto': 'CONTABILIDAD GERENCIAL', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>151</v>
       </c>
@@ -2100,19 +2111,19 @@
         <v>23</v>
       </c>
       <c r="J3" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H3&amp;", '"&amp;I$1&amp;"': '"&amp;I3&amp;"', '"&amp;C$1&amp;"': "&amp;C3&amp;", '"&amp;D$1&amp;"': "&amp;D3&amp;", '"&amp;E$1&amp;"': '"&amp;E3&amp;"', '"&amp;F$1&amp;"': '"&amp;F3&amp;"', '"&amp;G$1&amp;"':"&amp;G3&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 21, 'subtipo': 'generales', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'I. DATOS GENERALES', 'offset':1}, </v>
       </c>
       <c r="K3" s="2" t="str">
-        <f>IF(B2=B3,CONCATENATE(K2,J3),J3)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 21, 'subtipo': 'generales', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'I. DATOS GENERALES', 'offset':1}, </v>
       </c>
       <c r="L3" s="11" t="str">
-        <f>IF(B3=B4,"","{'"&amp;B$1&amp;"': "&amp;B3&amp;", 'editing': false, 'tipo': '"&amp;A3&amp;"', 'data': "&amp;"["&amp;K3&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 2, 'editing': false, 'tipo': 'titulo1', 'data': [{ 'reg': 21, 'subtipo': 'generales', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'I. DATOS GENERALES', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -2139,19 +2150,19 @@
         <v>35</v>
       </c>
       <c r="J4" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H4&amp;", '"&amp;I$1&amp;"': '"&amp;I4&amp;"', '"&amp;C$1&amp;"': "&amp;C4&amp;", '"&amp;D$1&amp;"': "&amp;D4&amp;", '"&amp;E$1&amp;"': '"&amp;E4&amp;"', '"&amp;F$1&amp;"': '"&amp;F4&amp;"', '"&amp;G$1&amp;"':"&amp;G4&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 35, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Código:', 'offset':2}, </v>
       </c>
       <c r="K4" s="2" t="str">
-        <f>IF(B3=B4,CONCATENATE(K3,J4),J4)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 35, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Código:', 'offset':2}, </v>
       </c>
       <c r="L4" s="11" t="str">
-        <f>IF(B4=B5,"","{'"&amp;B$1&amp;"': "&amp;B4&amp;", 'editing': false, 'tipo': '"&amp;A4&amp;"', 'data': "&amp;"["&amp;K4&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -2178,19 +2189,19 @@
         <v>85</v>
       </c>
       <c r="J5" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H5&amp;", '"&amp;I$1&amp;"': '"&amp;I5&amp;"', '"&amp;C$1&amp;"': "&amp;C5&amp;", '"&amp;D$1&amp;"': "&amp;D5&amp;", '"&amp;E$1&amp;"': '"&amp;E5&amp;"', '"&amp;F$1&amp;"': '"&amp;F5&amp;"', '"&amp;G$1&amp;"':"&amp;G5&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 85, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '100048', 'offset':1}, </v>
       </c>
       <c r="K5" s="2" t="str">
-        <f>IF(B4=B5,CONCATENATE(K4,J5),J5)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 35, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Código:', 'offset':2}, { 'reg': 85, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '100048', 'offset':1}, </v>
       </c>
       <c r="L5" s="11" t="str">
-        <f>IF(B5=B6,"","{'"&amp;B$1&amp;"': "&amp;B5&amp;", 'editing': false, 'tipo': '"&amp;A5&amp;"', 'data': "&amp;"["&amp;K5&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 3, 'editing': false, 'tipo': 'generales', 'data': [{ 'reg': 35, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Código:', 'offset':2}, { 'reg': 85, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '100048', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2217,19 +2228,19 @@
         <v>130</v>
       </c>
       <c r="J6" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H6&amp;", '"&amp;I$1&amp;"': '"&amp;I6&amp;"', '"&amp;C$1&amp;"': "&amp;C6&amp;", '"&amp;D$1&amp;"': "&amp;D6&amp;", '"&amp;E$1&amp;"': '"&amp;E6&amp;"', '"&amp;F$1&amp;"': '"&amp;F6&amp;"', '"&amp;G$1&amp;"':"&amp;G6&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 130, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Pre‐ Requisito :', 'offset':2}, </v>
       </c>
       <c r="K6" s="2" t="str">
-        <f>IF(B5=B6,CONCATENATE(K5,J6),J6)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 130, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Pre‐ Requisito :', 'offset':2}, </v>
       </c>
       <c r="L6" s="11" t="str">
-        <f>IF(B6=B7,"","{'"&amp;B$1&amp;"': "&amp;B6&amp;", 'editing': false, 'tipo': '"&amp;A6&amp;"', 'data': "&amp;"["&amp;K6&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2256,19 +2267,19 @@
         <v>7</v>
       </c>
       <c r="J7" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H7&amp;", '"&amp;I$1&amp;"': '"&amp;I7&amp;"', '"&amp;C$1&amp;"': "&amp;C7&amp;", '"&amp;D$1&amp;"': "&amp;D7&amp;", '"&amp;E$1&amp;"': '"&amp;E7&amp;"', '"&amp;F$1&amp;"': '"&amp;F7&amp;"', '"&amp;G$1&amp;"':"&amp;G7&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 7, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': 'Contabilidad General', 'offset':1}, </v>
       </c>
       <c r="K7" s="2" t="str">
-        <f>IF(B6=B7,CONCATENATE(K6,J7),J7)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 130, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Pre‐ Requisito :', 'offset':2}, { 'reg': 7, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': 'Contabilidad General', 'offset':1}, </v>
       </c>
       <c r="L7" s="11" t="str">
-        <f>IF(B7=B8,"","{'"&amp;B$1&amp;"': "&amp;B7&amp;", 'editing': false, 'tipo': '"&amp;A7&amp;"', 'data': "&amp;"["&amp;K7&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 4, 'editing': false, 'tipo': 'generales', 'data': [{ 'reg': 130, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Pre‐ Requisito :', 'offset':2}, { 'reg': 7, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': 'Contabilidad General', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -2295,19 +2306,19 @@
         <v>109</v>
       </c>
       <c r="J8" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H8&amp;", '"&amp;I$1&amp;"': '"&amp;I8&amp;"', '"&amp;C$1&amp;"': "&amp;C8&amp;", '"&amp;D$1&amp;"': "&amp;D8&amp;", '"&amp;E$1&amp;"': '"&amp;E8&amp;"', '"&amp;F$1&amp;"': '"&amp;F8&amp;"', '"&amp;G$1&amp;"':"&amp;G8&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 109, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Créditos : ', 'offset':2}, </v>
       </c>
       <c r="K8" s="2" t="str">
-        <f>IF(B7=B8,CONCATENATE(K7,J8),J8)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 109, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Créditos : ', 'offset':2}, </v>
       </c>
       <c r="L8" s="11" t="str">
-        <f>IF(B8=B9,"","{'"&amp;B$1&amp;"': "&amp;B8&amp;", 'editing': false, 'tipo': '"&amp;A8&amp;"', 'data': "&amp;"["&amp;K8&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -2334,19 +2345,19 @@
         <v>13</v>
       </c>
       <c r="J9" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H9&amp;", '"&amp;I$1&amp;"': '"&amp;I9&amp;"', '"&amp;C$1&amp;"': "&amp;C9&amp;", '"&amp;D$1&amp;"': "&amp;D9&amp;", '"&amp;E$1&amp;"': '"&amp;E9&amp;"', '"&amp;F$1&amp;"': '"&amp;F9&amp;"', '"&amp;G$1&amp;"':"&amp;G9&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 13, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '03', 'offset':1}, </v>
       </c>
       <c r="K9" s="2" t="str">
-        <f>IF(B8=B9,CONCATENATE(K8,J9),J9)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 109, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Créditos : ', 'offset':2}, { 'reg': 13, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '03', 'offset':1}, </v>
       </c>
       <c r="L9" s="11" t="str">
-        <f>IF(B9=B10,"","{'"&amp;B$1&amp;"': "&amp;B9&amp;", 'editing': false, 'tipo': '"&amp;A9&amp;"', 'data': "&amp;"["&amp;K9&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 5, 'editing': false, 'tipo': 'generales', 'data': [{ 'reg': 109, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Créditos : ', 'offset':2}, { 'reg': 13, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '03', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -2373,19 +2384,19 @@
         <v>128</v>
       </c>
       <c r="J10" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H10&amp;", '"&amp;I$1&amp;"': '"&amp;I10&amp;"', '"&amp;C$1&amp;"': "&amp;C10&amp;", '"&amp;D$1&amp;"': "&amp;D10&amp;", '"&amp;E$1&amp;"': '"&amp;E10&amp;"', '"&amp;F$1&amp;"': '"&amp;F10&amp;"', '"&amp;G$1&amp;"':"&amp;G10&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 128, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Horas :', 'offset':2}, </v>
       </c>
       <c r="K10" s="2" t="str">
-        <f>IF(B9=B10,CONCATENATE(K9,J10),J10)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 128, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Horas :', 'offset':2}, </v>
       </c>
       <c r="L10" s="11" t="str">
-        <f>IF(B10=B11,"","{'"&amp;B$1&amp;"': "&amp;B10&amp;", 'editing': false, 'tipo': '"&amp;A10&amp;"', 'data': "&amp;"["&amp;K10&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -2412,19 +2423,19 @@
         <v>91</v>
       </c>
       <c r="J11" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H11&amp;", '"&amp;I$1&amp;"': '"&amp;I11&amp;"', '"&amp;C$1&amp;"': "&amp;C11&amp;", '"&amp;D$1&amp;"': "&amp;D11&amp;", '"&amp;E$1&amp;"': '"&amp;E11&amp;"', '"&amp;F$1&amp;"': '"&amp;F11&amp;"', '"&amp;G$1&amp;"':"&amp;G11&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 91, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '04 horas', 'offset':1}, </v>
       </c>
       <c r="K11" s="2" t="str">
-        <f>IF(B10=B11,CONCATENATE(K10,J11),J11)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 128, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Horas :', 'offset':2}, { 'reg': 91, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '04 horas', 'offset':1}, </v>
       </c>
       <c r="L11" s="11" t="str">
-        <f>IF(B11=B12,"","{'"&amp;B$1&amp;"': "&amp;B11&amp;", 'editing': false, 'tipo': '"&amp;A11&amp;"', 'data': "&amp;"["&amp;K11&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 6, 'editing': false, 'tipo': 'generales', 'data': [{ 'reg': 128, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Horas :', 'offset':2}, { 'reg': 91, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '04 horas', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -2451,19 +2462,19 @@
         <v>24</v>
       </c>
       <c r="J12" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H12&amp;", '"&amp;I$1&amp;"': '"&amp;I12&amp;"', '"&amp;C$1&amp;"': "&amp;C12&amp;", '"&amp;D$1&amp;"': "&amp;D12&amp;", '"&amp;E$1&amp;"': '"&amp;E12&amp;"', '"&amp;F$1&amp;"': '"&amp;F12&amp;"', '"&amp;G$1&amp;"':"&amp;G12&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 24, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Semestre académico : ', 'offset':2}, </v>
       </c>
       <c r="K12" s="2" t="str">
-        <f>IF(B11=B12,CONCATENATE(K11,J12),J12)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 24, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Semestre académico : ', 'offset':2}, </v>
       </c>
       <c r="L12" s="11" t="str">
-        <f>IF(B12=B13,"","{'"&amp;B$1&amp;"': "&amp;B12&amp;", 'editing': false, 'tipo': '"&amp;A12&amp;"', 'data': "&amp;"["&amp;K12&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -2490,19 +2501,19 @@
         <v>86</v>
       </c>
       <c r="J13" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H13&amp;", '"&amp;I$1&amp;"': '"&amp;I13&amp;"', '"&amp;C$1&amp;"': "&amp;C13&amp;", '"&amp;D$1&amp;"': "&amp;D13&amp;", '"&amp;E$1&amp;"': '"&amp;E13&amp;"', '"&amp;F$1&amp;"': '"&amp;F13&amp;"', '"&amp;G$1&amp;"':"&amp;G13&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 86, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '2017‐ I', 'offset':1}, </v>
       </c>
       <c r="K13" s="2" t="str">
-        <f>IF(B12=B13,CONCATENATE(K12,J13),J13)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 24, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Semestre académico : ', 'offset':2}, { 'reg': 86, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '2017‐ I', 'offset':1}, </v>
       </c>
       <c r="L13" s="11" t="str">
-        <f>IF(B13=B14,"","{'"&amp;B$1&amp;"': "&amp;B13&amp;", 'editing': false, 'tipo': '"&amp;A13&amp;"', 'data': "&amp;"["&amp;K13&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 7, 'editing': false, 'tipo': 'generales', 'data': [{ 'reg': 24, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Semestre académico : ', 'offset':2}, { 'reg': 86, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': '2017‐ I', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -2529,19 +2540,19 @@
         <v>81</v>
       </c>
       <c r="J14" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H14&amp;", '"&amp;I$1&amp;"': '"&amp;I14&amp;"', '"&amp;C$1&amp;"': "&amp;C14&amp;", '"&amp;D$1&amp;"': "&amp;D14&amp;", '"&amp;E$1&amp;"': '"&amp;E14&amp;"', '"&amp;F$1&amp;"': '"&amp;F14&amp;"', '"&amp;G$1&amp;"':"&amp;G14&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 81, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Ciclo :', 'offset':2}, </v>
       </c>
       <c r="K14" s="2" t="str">
-        <f>IF(B13=B14,CONCATENATE(K13,J14),J14)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 81, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Ciclo :', 'offset':2}, </v>
       </c>
       <c r="L14" s="11" t="str">
-        <f>IF(B14=B15,"","{'"&amp;B$1&amp;"': "&amp;B14&amp;", 'editing': false, 'tipo': '"&amp;A14&amp;"', 'data': "&amp;"["&amp;K14&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2568,19 +2579,19 @@
         <v>103</v>
       </c>
       <c r="J15" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H15&amp;", '"&amp;I$1&amp;"': '"&amp;I15&amp;"', '"&amp;C$1&amp;"': "&amp;C15&amp;", '"&amp;D$1&amp;"': "&amp;D15&amp;", '"&amp;E$1&amp;"': '"&amp;E15&amp;"', '"&amp;F$1&amp;"': '"&amp;F15&amp;"', '"&amp;G$1&amp;"':"&amp;G15&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 103, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': 'III', 'offset':1}, </v>
       </c>
       <c r="K15" s="2" t="str">
-        <f>IF(B14=B15,CONCATENATE(K14,J15),J15)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 81, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Ciclo :', 'offset':2}, { 'reg': 103, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': 'III', 'offset':1}, </v>
       </c>
       <c r="L15" s="11" t="str">
-        <f>IF(B15=B16,"","{'"&amp;B$1&amp;"': "&amp;B15&amp;", 'editing': false, 'tipo': '"&amp;A15&amp;"', 'data': "&amp;"["&amp;K15&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 8, 'editing': false, 'tipo': 'generales', 'data': [{ 'reg': 81, 'subtipo': '', 'col': 2, 'cols': 2, 'align': 'left', 'texto': 'Ciclo :', 'offset':2}, { 'reg': 103, 'subtipo': '', 'col': 3, 'cols': 2, 'align': 'left', 'texto': 'III', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>151</v>
       </c>
@@ -2610,19 +2621,19 @@
         <v>153</v>
       </c>
       <c r="J16" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H16&amp;", '"&amp;I$1&amp;"': '"&amp;I16&amp;"', '"&amp;C$1&amp;"': "&amp;C16&amp;", '"&amp;D$1&amp;"': "&amp;D16&amp;", '"&amp;E$1&amp;"': '"&amp;E16&amp;"', '"&amp;F$1&amp;"': '"&amp;F16&amp;"', '"&amp;G$1&amp;"':"&amp;G16&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 45, 'subtipo': 'sumillas', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'II. SUMILLA', 'offset':1}, </v>
       </c>
       <c r="K16" s="2" t="str">
-        <f>IF(B15=B16,CONCATENATE(K15,J16),J16)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 45, 'subtipo': 'sumillas', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'II. SUMILLA', 'offset':1}, </v>
       </c>
       <c r="L16" s="11" t="str">
-        <f>IF(B16=B17,"","{'"&amp;B$1&amp;"': "&amp;B16&amp;", 'editing': false, 'tipo': '"&amp;A16&amp;"', 'data': "&amp;"["&amp;K16&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 9, 'editing': false, 'tipo': 'titulo1', 'data': [{ 'reg': 45, 'subtipo': 'sumillas', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'II. SUMILLA', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>153</v>
       </c>
@@ -2649,19 +2660,19 @@
         <v>36</v>
       </c>
       <c r="J17" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H17&amp;", '"&amp;I$1&amp;"': '"&amp;I17&amp;"', '"&amp;C$1&amp;"': "&amp;C17&amp;", '"&amp;D$1&amp;"': "&amp;D17&amp;", '"&amp;E$1&amp;"': '"&amp;E17&amp;"', '"&amp;F$1&amp;"': '"&amp;F17&amp;"', '"&amp;G$1&amp;"':"&amp;G17&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 36, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'justify', 'texto': 'El curso tiene como propósito integrar las teorías, las técnicas y las herramientas adquiridas en las materias de contabilidad general y administración que le permita llegar al alumno a desarrollar las habilidades de análisis, integración de la información para la construcción de propuestas y soluciones que llevan al logro de los objetivos de la organización. Se pondrá énfasis en el análisis financiero de los estados financieros y su relación con los costos empresariales.', 'offset':1}, </v>
       </c>
       <c r="K17" s="2" t="str">
-        <f>IF(B16=B17,CONCATENATE(K16,J17),J17)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 36, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'justify', 'texto': 'El curso tiene como propósito integrar las teorías, las técnicas y las herramientas adquiridas en las materias de contabilidad general y administración que le permita llegar al alumno a desarrollar las habilidades de análisis, integración de la información para la construcción de propuestas y soluciones que llevan al logro de los objetivos de la organización. Se pondrá énfasis en el análisis financiero de los estados financieros y su relación con los costos empresariales.', 'offset':1}, </v>
       </c>
       <c r="L17" s="11" t="str">
-        <f>IF(B17=B18,"","{'"&amp;B$1&amp;"': "&amp;B17&amp;", 'editing': false, 'tipo': '"&amp;A17&amp;"', 'data': "&amp;"["&amp;K17&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 10, 'editing': false, 'tipo': 'sumillas', 'data': [{ 'reg': 36, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'justify', 'texto': 'El curso tiene como propósito integrar las teorías, las técnicas y las herramientas adquiridas en las materias de contabilidad general y administración que le permita llegar al alumno a desarrollar las habilidades de análisis, integración de la información para la construcción de propuestas y soluciones que llevan al logro de los objetivos de la organización. Se pondrá énfasis en el análisis financiero de los estados financieros y su relación con los costos empresariales.', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>151</v>
       </c>
@@ -2691,19 +2702,19 @@
         <v>155</v>
       </c>
       <c r="J18" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H18&amp;", '"&amp;I$1&amp;"': '"&amp;I18&amp;"', '"&amp;C$1&amp;"': "&amp;C18&amp;", '"&amp;D$1&amp;"': "&amp;D18&amp;", '"&amp;E$1&amp;"': '"&amp;E18&amp;"', '"&amp;F$1&amp;"': '"&amp;F18&amp;"', '"&amp;G$1&amp;"':"&amp;G18&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 82, 'subtipo': 'competencias', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'III. SISTEMA DE COMPETENCIAS', 'offset':1}, </v>
       </c>
       <c r="K18" s="2" t="str">
-        <f>IF(B17=B18,CONCATENATE(K17,J18),J18)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 82, 'subtipo': 'competencias', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'III. SISTEMA DE COMPETENCIAS', 'offset':1}, </v>
       </c>
       <c r="L18" s="11" t="str">
-        <f>IF(B18=B19,"","{'"&amp;B$1&amp;"': "&amp;B18&amp;", 'editing': false, 'tipo': '"&amp;A18&amp;"', 'data': "&amp;"["&amp;K18&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 11, 'editing': false, 'tipo': 'titulo1', 'data': [{ 'reg': 82, 'subtipo': 'competencias', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'III. SISTEMA DE COMPETENCIAS', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>156</v>
       </c>
@@ -2730,19 +2741,19 @@
         <v>37</v>
       </c>
       <c r="J19" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H19&amp;", '"&amp;I$1&amp;"': '"&amp;I19&amp;"', '"&amp;C$1&amp;"': "&amp;C19&amp;", '"&amp;D$1&amp;"': "&amp;D19&amp;", '"&amp;E$1&amp;"': '"&amp;E19&amp;"', '"&amp;F$1&amp;"': '"&amp;F19&amp;"', '"&amp;G$1&amp;"':"&amp;G19&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 37, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'COMPETENCIAS GENERALES', 'offset':1}, </v>
       </c>
       <c r="K19" s="2" t="str">
-        <f>IF(B18=B19,CONCATENATE(K18,J19),J19)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 37, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'COMPETENCIAS GENERALES', 'offset':1}, </v>
       </c>
       <c r="L19" s="11" t="str">
-        <f>IF(B19=B20,"","{'"&amp;B$1&amp;"': "&amp;B19&amp;", 'editing': false, 'tipo': '"&amp;A19&amp;"', 'data': "&amp;"["&amp;K19&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 12, 'editing': false, 'tipo': 'titulo2', 'data': [{ 'reg': 37, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'COMPETENCIAS GENERALES', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>155</v>
       </c>
@@ -2770,24 +2781,24 @@
         <v>10</v>
       </c>
       <c r="J20" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H20&amp;", '"&amp;I$1&amp;"': '"&amp;I20&amp;"', '"&amp;C$1&amp;"': "&amp;C20&amp;", '"&amp;D$1&amp;"': "&amp;D20&amp;", '"&amp;E$1&amp;"': '"&amp;E20&amp;"', '"&amp;F$1&amp;"': '"&amp;F20&amp;"', '"&amp;G$1&amp;"':"&amp;G20&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 10, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Comprende el papel de la información contable en los Negocios. Relación entre la contabilidad y la Administración y la toma de decisiones.', 'offset':2}, </v>
       </c>
       <c r="K20" s="2" t="str">
-        <f>IF(B19=B20,CONCATENATE(K19,J20),J20)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 10, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Comprende el papel de la información contable en los Negocios. Relación entre la contabilidad y la Administración y la toma de decisiones.', 'offset':2}, </v>
       </c>
       <c r="L20" s="11" t="str">
-        <f>IF(B20=B21,"","{'"&amp;B$1&amp;"': "&amp;B20&amp;", 'editing': false, 'tipo': '"&amp;A20&amp;"', 'data': "&amp;"["&amp;K20&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 13, 'editing': false, 'tipo': 'competencias', 'data': [{ 'reg': 10, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Comprende el papel de la información contable en los Negocios. Relación entre la contabilidad y la Administración y la toma de decisiones.', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B33" si="1">+B20+1</f>
+        <f t="shared" ref="B21:B33" si="4">+B20+1</f>
         <v>14</v>
       </c>
       <c r="C21" s="2">
@@ -2810,24 +2821,24 @@
         <v>13</v>
       </c>
       <c r="J21" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H21&amp;", '"&amp;I$1&amp;"': '"&amp;I21&amp;"', '"&amp;C$1&amp;"': "&amp;C21&amp;", '"&amp;D$1&amp;"': "&amp;D21&amp;", '"&amp;E$1&amp;"': '"&amp;E21&amp;"', '"&amp;F$1&amp;"': '"&amp;F21&amp;"', '"&amp;G$1&amp;"':"&amp;G21&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 13, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Conoce y ejecuta los Estados Financieros de una empresa comercial, industrial y de servicios.', 'offset':2}, </v>
       </c>
       <c r="K21" s="2" t="str">
-        <f>IF(B20=B21,CONCATENATE(K20,J21),J21)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 13, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Conoce y ejecuta los Estados Financieros de una empresa comercial, industrial y de servicios.', 'offset':2}, </v>
       </c>
       <c r="L21" s="11" t="str">
-        <f>IF(B21=B22,"","{'"&amp;B$1&amp;"': "&amp;B21&amp;", 'editing': false, 'tipo': '"&amp;A21&amp;"', 'data': "&amp;"["&amp;K21&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 14, 'editing': false, 'tipo': 'competencias', 'data': [{ 'reg': 13, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Conoce y ejecuta los Estados Financieros de una empresa comercial, industrial y de servicios.', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="C22" s="2">
@@ -2850,24 +2861,24 @@
         <v>81</v>
       </c>
       <c r="J22" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H22&amp;", '"&amp;I$1&amp;"': '"&amp;I22&amp;"', '"&amp;C$1&amp;"': "&amp;C22&amp;", '"&amp;D$1&amp;"': "&amp;D22&amp;", '"&amp;E$1&amp;"': '"&amp;E22&amp;"', '"&amp;F$1&amp;"': '"&amp;F22&amp;"', '"&amp;G$1&amp;"':"&amp;G22&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 81, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Toma de decisiones, en base a un análisis financiero, dentro de las funciones de operación, inversión y financiamiento y análisis de los costos.', 'offset':2}, </v>
       </c>
       <c r="K22" s="2" t="str">
-        <f>IF(B21=B22,CONCATENATE(K21,J22),J22)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 81, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Toma de decisiones, en base a un análisis financiero, dentro de las funciones de operación, inversión y financiamiento y análisis de los costos.', 'offset':2}, </v>
       </c>
       <c r="L22" s="11" t="str">
-        <f>IF(B22=B23,"","{'"&amp;B$1&amp;"': "&amp;B22&amp;", 'editing': false, 'tipo': '"&amp;A22&amp;"', 'data': "&amp;"["&amp;K22&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 15, 'editing': false, 'tipo': 'competencias', 'data': [{ 'reg': 81, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Toma de decisiones, en base a un análisis financiero, dentro de las funciones de operación, inversión y financiamiento y análisis de los costos.', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="C23" s="2">
@@ -2890,24 +2901,24 @@
         <v>41</v>
       </c>
       <c r="J23" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H23&amp;", '"&amp;I$1&amp;"': '"&amp;I23&amp;"', '"&amp;C$1&amp;"': "&amp;C23&amp;", '"&amp;D$1&amp;"': "&amp;D23&amp;", '"&amp;E$1&amp;"': '"&amp;E23&amp;"', '"&amp;F$1&amp;"': '"&amp;F23&amp;"', '"&amp;G$1&amp;"':"&amp;G23&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 41, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Planifica la gestión de la empresa a futuro.', 'offset':2}, </v>
       </c>
       <c r="K23" s="2" t="str">
-        <f>IF(B22=B23,CONCATENATE(K22,J23),J23)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 41, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Planifica la gestión de la empresa a futuro.', 'offset':2}, </v>
       </c>
       <c r="L23" s="11" t="str">
-        <f>IF(B23=B24,"","{'"&amp;B$1&amp;"': "&amp;B23&amp;", 'editing': false, 'tipo': '"&amp;A23&amp;"', 'data': "&amp;"["&amp;K23&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 16, 'editing': false, 'tipo': 'competencias', 'data': [{ 'reg': 41, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Planifica la gestión de la empresa a futuro.', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="C24" s="2">
@@ -2930,24 +2941,24 @@
         <v>77</v>
       </c>
       <c r="J24" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H24&amp;", '"&amp;I$1&amp;"': '"&amp;I24&amp;"', '"&amp;C$1&amp;"': "&amp;C24&amp;", '"&amp;D$1&amp;"': "&amp;D24&amp;", '"&amp;E$1&amp;"': '"&amp;E24&amp;"', '"&amp;F$1&amp;"': '"&amp;F24&amp;"', '"&amp;G$1&amp;"':"&amp;G24&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 77, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Capacidad de trabajo en equipo.', 'offset':2}, </v>
       </c>
       <c r="K24" s="2" t="str">
-        <f>IF(B23=B24,CONCATENATE(K23,J24),J24)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 77, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Capacidad de trabajo en equipo.', 'offset':2}, </v>
       </c>
       <c r="L24" s="11" t="str">
-        <f>IF(B24=B25,"","{'"&amp;B$1&amp;"': "&amp;B24&amp;", 'editing': false, 'tipo': '"&amp;A24&amp;"', 'data': "&amp;"["&amp;K24&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 17, 'editing': false, 'tipo': 'competencias', 'data': [{ 'reg': 77, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Capacidad de trabajo en equipo.', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="C25" s="2">
@@ -2970,24 +2981,24 @@
         <v>9</v>
       </c>
       <c r="J25" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H25&amp;", '"&amp;I$1&amp;"': '"&amp;I25&amp;"', '"&amp;C$1&amp;"': "&amp;C25&amp;", '"&amp;D$1&amp;"': "&amp;D25&amp;", '"&amp;E$1&amp;"': '"&amp;E25&amp;"', '"&amp;F$1&amp;"': '"&amp;F25&amp;"', '"&amp;G$1&amp;"':"&amp;G25&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 9, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'COMPETENCIAS ESPECÍFICAS', 'offset':1}, </v>
       </c>
       <c r="K25" s="2" t="str">
-        <f>IF(B24=B25,CONCATENATE(K24,J25),J25)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 9, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'COMPETENCIAS ESPECÍFICAS', 'offset':1}, </v>
       </c>
       <c r="L25" s="11" t="str">
-        <f>IF(B25=B26,"","{'"&amp;B$1&amp;"': "&amp;B25&amp;", 'editing': false, 'tipo': '"&amp;A25&amp;"', 'data': "&amp;"["&amp;K25&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 18, 'editing': false, 'tipo': 'titulo2', 'data': [{ 'reg': 9, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'COMPETENCIAS ESPECÍFICAS', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="C26" s="2">
@@ -3010,24 +3021,24 @@
         <v>84</v>
       </c>
       <c r="J26" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H26&amp;", '"&amp;I$1&amp;"': '"&amp;I26&amp;"', '"&amp;C$1&amp;"': "&amp;C26&amp;", '"&amp;D$1&amp;"': "&amp;D26&amp;", '"&amp;E$1&amp;"': '"&amp;E26&amp;"', '"&amp;F$1&amp;"': '"&amp;F26&amp;"', '"&amp;G$1&amp;"':"&amp;G26&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 84, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Conoce, Analiza y describe las diferentes empresas que se desarrollan en nuestro país y la importancia que tiene en ellas la contabilidad gerencia, desde la óptica de los estados financieros: Estado de Situación Financiera y Estado de Resultados.', 'offset':2}, </v>
       </c>
       <c r="K26" s="2" t="str">
-        <f>IF(B25=B26,CONCATENATE(K25,J26),J26)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 84, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Conoce, Analiza y describe las diferentes empresas que se desarrollan en nuestro país y la importancia que tiene en ellas la contabilidad gerencia, desde la óptica de los estados financieros: Estado de Situación Financiera y Estado de Resultados.', 'offset':2}, </v>
       </c>
       <c r="L26" s="11" t="str">
-        <f>IF(B26=B27,"","{'"&amp;B$1&amp;"': "&amp;B26&amp;", 'editing': false, 'tipo': '"&amp;A26&amp;"', 'data': "&amp;"["&amp;K26&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 19, 'editing': false, 'tipo': 'competencias', 'data': [{ 'reg': 84, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Conoce, Analiza y describe las diferentes empresas que se desarrollan en nuestro país y la importancia que tiene en ellas la contabilidad gerencia, desde la óptica de los estados financieros: Estado de Situación Financiera y Estado de Resultados.', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="C27" s="2">
@@ -3050,24 +3061,24 @@
         <v>32</v>
       </c>
       <c r="J27" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H27&amp;", '"&amp;I$1&amp;"': '"&amp;I27&amp;"', '"&amp;C$1&amp;"': "&amp;C27&amp;", '"&amp;D$1&amp;"': "&amp;D27&amp;", '"&amp;E$1&amp;"': '"&amp;E27&amp;"', '"&amp;F$1&amp;"': '"&amp;F27&amp;"', '"&amp;G$1&amp;"':"&amp;G27&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 32, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Analiza y diagnostica los Estados financieros básicos de diferentes empresas, mediante el análisis vertical y horizontal así como los ratios financieros. ', 'offset':2}, </v>
       </c>
       <c r="K27" s="2" t="str">
-        <f>IF(B26=B27,CONCATENATE(K26,J27),J27)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 32, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Analiza y diagnostica los Estados financieros básicos de diferentes empresas, mediante el análisis vertical y horizontal así como los ratios financieros. ', 'offset':2}, </v>
       </c>
       <c r="L27" s="11" t="str">
-        <f>IF(B27=B28,"","{'"&amp;B$1&amp;"': "&amp;B27&amp;", 'editing': false, 'tipo': '"&amp;A27&amp;"', 'data': "&amp;"["&amp;K27&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 20, 'editing': false, 'tipo': 'competencias', 'data': [{ 'reg': 32, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Analiza y diagnostica los Estados financieros básicos de diferentes empresas, mediante el análisis vertical y horizontal así como los ratios financieros. ', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="C28" s="2">
@@ -3090,24 +3101,24 @@
         <v>111</v>
       </c>
       <c r="J28" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H28&amp;", '"&amp;I$1&amp;"': '"&amp;I28&amp;"', '"&amp;C$1&amp;"': "&amp;C28&amp;", '"&amp;D$1&amp;"': "&amp;D28&amp;", '"&amp;E$1&amp;"': '"&amp;E28&amp;"', '"&amp;F$1&amp;"': '"&amp;F28&amp;"', '"&amp;G$1&amp;"':"&amp;G28&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 111, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Desarrolla un plan financiero para una empresa: Presupuesto de ventas, Presupuesto de cobranzas, presupuesto de producción, presupuesto de compras, presupuesto de pagos, presupuesto de pagos, presupuesto de gastos, entre otros.', 'offset':2}, </v>
       </c>
       <c r="K28" s="2" t="str">
-        <f>IF(B27=B28,CONCATENATE(K27,J28),J28)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 111, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Desarrolla un plan financiero para una empresa: Presupuesto de ventas, Presupuesto de cobranzas, presupuesto de producción, presupuesto de compras, presupuesto de pagos, presupuesto de pagos, presupuesto de gastos, entre otros.', 'offset':2}, </v>
       </c>
       <c r="L28" s="11" t="str">
-        <f>IF(B28=B29,"","{'"&amp;B$1&amp;"': "&amp;B28&amp;", 'editing': false, 'tipo': '"&amp;A28&amp;"', 'data': "&amp;"["&amp;K28&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 21, 'editing': false, 'tipo': 'competencias', 'data': [{ 'reg': 111, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Desarrolla un plan financiero para una empresa: Presupuesto de ventas, Presupuesto de cobranzas, presupuesto de producción, presupuesto de compras, presupuesto de pagos, presupuesto de pagos, presupuesto de gastos, entre otros.', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="C29" s="2">
@@ -3130,24 +3141,24 @@
         <v>28</v>
       </c>
       <c r="J29" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H29&amp;", '"&amp;I$1&amp;"': '"&amp;I29&amp;"', '"&amp;C$1&amp;"': "&amp;C29&amp;", '"&amp;D$1&amp;"': "&amp;D29&amp;", '"&amp;E$1&amp;"': '"&amp;E29&amp;"', '"&amp;F$1&amp;"': '"&amp;F29&amp;"', '"&amp;G$1&amp;"':"&amp;G29&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 28, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Estudia la importancia de la estructura de costos de una empresa y su implicancia en la planificación financiera.', 'offset':2}, </v>
       </c>
       <c r="K29" s="2" t="str">
-        <f>IF(B28=B29,CONCATENATE(K28,J29),J29)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 28, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Estudia la importancia de la estructura de costos de una empresa y su implicancia en la planificación financiera.', 'offset':2}, </v>
       </c>
       <c r="L29" s="11" t="str">
-        <f>IF(B29=B30,"","{'"&amp;B$1&amp;"': "&amp;B29&amp;", 'editing': false, 'tipo': '"&amp;A29&amp;"', 'data': "&amp;"["&amp;K29&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 22, 'editing': false, 'tipo': 'competencias', 'data': [{ 'reg': 28, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Estudia la importancia de la estructura de costos de una empresa y su implicancia en la planificación financiera.', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="C30" s="2">
@@ -3170,24 +3181,24 @@
         <v>27</v>
       </c>
       <c r="J30" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H30&amp;", '"&amp;I$1&amp;"': '"&amp;I30&amp;"', '"&amp;C$1&amp;"': "&amp;C30&amp;", '"&amp;D$1&amp;"': "&amp;D30&amp;", '"&amp;E$1&amp;"': '"&amp;E30&amp;"', '"&amp;F$1&amp;"': '"&amp;F30&amp;"', '"&amp;G$1&amp;"':"&amp;G30&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 27, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Elabora estados financieros proyectados, para diagnosticar el futuro de la empresa.', 'offset':2}, </v>
       </c>
       <c r="K30" s="2" t="str">
-        <f>IF(B29=B30,CONCATENATE(K29,J30),J30)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 27, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Elabora estados financieros proyectados, para diagnosticar el futuro de la empresa.', 'offset':2}, </v>
       </c>
       <c r="L30" s="11" t="str">
-        <f>IF(B30=B31,"","{'"&amp;B$1&amp;"': "&amp;B30&amp;", 'editing': false, 'tipo': '"&amp;A30&amp;"', 'data': "&amp;"["&amp;K30&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 23, 'editing': false, 'tipo': 'competencias', 'data': [{ 'reg': 27, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'justify', 'texto': 'Elabora estados financieros proyectados, para diagnosticar el futuro de la empresa.', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="C31" s="2">
@@ -3213,24 +3224,24 @@
         <v>159</v>
       </c>
       <c r="J31" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H31&amp;", '"&amp;I$1&amp;"': '"&amp;I31&amp;"', '"&amp;C$1&amp;"': "&amp;C31&amp;", '"&amp;D$1&amp;"': "&amp;D31&amp;", '"&amp;E$1&amp;"': '"&amp;E31&amp;"', '"&amp;F$1&amp;"': '"&amp;F31&amp;"', '"&amp;G$1&amp;"':"&amp;G31&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 126, 'subtipo': 'contenidos', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'IV. PROGRAMACIÓN DE CONTENIDOS', 'offset':1}, </v>
       </c>
       <c r="K31" s="2" t="str">
-        <f>IF(B30=B31,CONCATENATE(K30,J31),J31)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 126, 'subtipo': 'contenidos', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'IV. PROGRAMACIÓN DE CONTENIDOS', 'offset':1}, </v>
       </c>
       <c r="L31" s="11" t="str">
-        <f>IF(B31=B32,"","{'"&amp;B$1&amp;"': "&amp;B31&amp;", 'editing': false, 'tipo': '"&amp;A31&amp;"', 'data': "&amp;"["&amp;K31&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 24, 'editing': false, 'tipo': 'titulo1', 'data': [{ 'reg': 126, 'subtipo': 'contenidos', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'IV. PROGRAMACIÓN DE CONTENIDOS', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="C32" s="2">
@@ -3253,24 +3264,24 @@
         <v>22</v>
       </c>
       <c r="J32" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H32&amp;", '"&amp;I$1&amp;"': '"&amp;I32&amp;"', '"&amp;C$1&amp;"': "&amp;C32&amp;", '"&amp;D$1&amp;"': "&amp;D32&amp;", '"&amp;E$1&amp;"': '"&amp;E32&amp;"', '"&amp;F$1&amp;"': '"&amp;F32&amp;"', '"&amp;G$1&amp;"':"&amp;G32&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 22, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'center', 'texto': 'UNIDAD I: LA CONTABILIDAD GERENCIAL.', 'offset':1}, </v>
       </c>
       <c r="K32" s="2" t="str">
-        <f>IF(B31=B32,CONCATENATE(K31,J32),J32)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 22, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'center', 'texto': 'UNIDAD I: LA CONTABILIDAD GERENCIAL.', 'offset':1}, </v>
       </c>
       <c r="L32" s="11" t="str">
-        <f>IF(B32=B33,"","{'"&amp;B$1&amp;"': "&amp;B32&amp;", 'editing': false, 'tipo': '"&amp;A32&amp;"', 'data': "&amp;"["&amp;K32&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v>{'row': 25, 'editing': false, 'tipo': 'unidades', 'data': [{ 'reg': 22, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'center', 'texto': 'UNIDAD I: LA CONTABILIDAD GERENCIAL.', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="C33" s="2">
@@ -3293,19 +3304,19 @@
         <v>35</v>
       </c>
       <c r="J33" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H33&amp;", '"&amp;I$1&amp;"': '"&amp;I33&amp;"', '"&amp;C$1&amp;"': "&amp;C33&amp;", '"&amp;D$1&amp;"': "&amp;D33&amp;", '"&amp;E$1&amp;"': '"&amp;E33&amp;"', '"&amp;F$1&amp;"': '"&amp;F33&amp;"', '"&amp;G$1&amp;"':"&amp;G33&amp;"}, "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ 'reg': 35, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, </v>
       </c>
       <c r="K33" s="2" t="str">
-        <f>IF(B32=B33,CONCATENATE(K32,J33),J33)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ 'reg': 35, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, </v>
       </c>
       <c r="L33" s="11" t="str">
-        <f>IF(B33=B34,"","{'"&amp;B$1&amp;"': "&amp;B33&amp;", 'editing': false, 'tipo': '"&amp;A33&amp;"', 'data': "&amp;"["&amp;K33&amp;"],  },")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>157</v>
       </c>
@@ -3326,26 +3337,26 @@
         <v>60</v>
       </c>
       <c r="G34" s="7">
-        <f t="shared" ref="G34:G65" si="2">IF(B33=B34,1,C34)</f>
+        <f t="shared" ref="G34:G65" si="5">IF(B33=B34,1,C34)</f>
         <v>1</v>
       </c>
       <c r="H34" s="14">
         <v>48</v>
       </c>
       <c r="J34" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H34&amp;", '"&amp;I$1&amp;"': '"&amp;I34&amp;"', '"&amp;C$1&amp;"': "&amp;C34&amp;", '"&amp;D$1&amp;"': "&amp;D34&amp;", '"&amp;E$1&amp;"': '"&amp;E34&amp;"', '"&amp;F$1&amp;"': '"&amp;F34&amp;"', '"&amp;G$1&amp;"':"&amp;G34&amp;"}, "</f>
+        <f t="shared" ref="J34:J65" si="6">+"{ '"&amp;H$1&amp;"': "&amp;H34&amp;", '"&amp;I$1&amp;"': '"&amp;I34&amp;"', '"&amp;C$1&amp;"': "&amp;C34&amp;", '"&amp;D$1&amp;"': "&amp;D34&amp;", '"&amp;E$1&amp;"': '"&amp;E34&amp;"', '"&amp;F$1&amp;"': '"&amp;F34&amp;"', '"&amp;G$1&amp;"':"&amp;G34&amp;"}, "</f>
         <v xml:space="preserve">{ 'reg': 48, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'center', 'texto': 'CONCEPTUAL', 'offset':1}, </v>
       </c>
       <c r="K34" s="2" t="str">
-        <f>IF(B33=B34,CONCATENATE(K33,J34),J34)</f>
+        <f t="shared" ref="K34:K65" si="7">IF(B33=B34,CONCATENATE(K33,J34),J34)</f>
         <v xml:space="preserve">{ 'reg': 35, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, { 'reg': 48, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'center', 'texto': 'CONCEPTUAL', 'offset':1}, </v>
       </c>
       <c r="L34" s="11" t="str">
-        <f>IF(B34=B35,"","{'"&amp;B$1&amp;"': "&amp;B34&amp;", 'editing': false, 'tipo': '"&amp;A34&amp;"', 'data': "&amp;"["&amp;K34&amp;"],  },")</f>
+        <f t="shared" ref="L34:L65" si="8">IF(B34=B35,"","{'"&amp;B$1&amp;"': "&amp;B34&amp;", 'editing': false, 'tipo': '"&amp;A34&amp;"', 'data': "&amp;"["&amp;K34&amp;"],  },")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>157</v>
       </c>
@@ -3366,26 +3377,26 @@
         <v>61</v>
       </c>
       <c r="G35" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H35" s="14">
         <v>14</v>
       </c>
       <c r="J35" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H35&amp;", '"&amp;I$1&amp;"': '"&amp;I35&amp;"', '"&amp;C$1&amp;"': "&amp;C35&amp;", '"&amp;D$1&amp;"': "&amp;D35&amp;", '"&amp;E$1&amp;"': '"&amp;E35&amp;"', '"&amp;F$1&amp;"': '"&amp;F35&amp;"', '"&amp;G$1&amp;"':"&amp;G35&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 14, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'center', 'texto': 'PROCEDIMENTAL', 'offset':1}, </v>
       </c>
       <c r="K35" s="2" t="str">
-        <f>IF(B34=B35,CONCATENATE(K34,J35),J35)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 35, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, { 'reg': 48, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'center', 'texto': 'CONCEPTUAL', 'offset':1}, { 'reg': 14, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'center', 'texto': 'PROCEDIMENTAL', 'offset':1}, </v>
       </c>
       <c r="L35" s="11" t="str">
-        <f>IF(B35=B36,"","{'"&amp;B$1&amp;"': "&amp;B35&amp;", 'editing': false, 'tipo': '"&amp;A35&amp;"', 'data': "&amp;"["&amp;K35&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>157</v>
       </c>
@@ -3406,26 +3417,26 @@
         <v>62</v>
       </c>
       <c r="G36" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H36" s="14">
         <v>25</v>
       </c>
       <c r="J36" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H36&amp;", '"&amp;I$1&amp;"': '"&amp;I36&amp;"', '"&amp;C$1&amp;"': "&amp;C36&amp;", '"&amp;D$1&amp;"': "&amp;D36&amp;", '"&amp;E$1&amp;"': '"&amp;E36&amp;"', '"&amp;F$1&amp;"': '"&amp;F36&amp;"', '"&amp;G$1&amp;"':"&amp;G36&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 25, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'center', 'texto': 'ACTIVIDAD DE APRENDIZAJE', 'offset':1}, </v>
       </c>
       <c r="K36" s="2" t="str">
-        <f>IF(B35=B36,CONCATENATE(K35,J36),J36)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 35, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, { 'reg': 48, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'center', 'texto': 'CONCEPTUAL', 'offset':1}, { 'reg': 14, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'center', 'texto': 'PROCEDIMENTAL', 'offset':1}, { 'reg': 25, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'center', 'texto': 'ACTIVIDAD DE APRENDIZAJE', 'offset':1}, </v>
       </c>
       <c r="L36" s="11" t="str">
-        <f>IF(B36=B37,"","{'"&amp;B$1&amp;"': "&amp;B36&amp;", 'editing': false, 'tipo': '"&amp;A36&amp;"', 'data': "&amp;"["&amp;K36&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 26, 'editing': false, 'tipo': 'titulo3', 'data': [{ 'reg': 35, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, { 'reg': 48, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'center', 'texto': 'CONCEPTUAL', 'offset':1}, { 'reg': 14, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'center', 'texto': 'PROCEDIMENTAL', 'offset':1}, { 'reg': 25, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'center', 'texto': 'ACTIVIDAD DE APRENDIZAJE', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>159</v>
       </c>
@@ -3446,26 +3457,26 @@
         <v>1</v>
       </c>
       <c r="G37" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H37" s="14">
         <v>99</v>
       </c>
       <c r="J37" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H37&amp;", '"&amp;I$1&amp;"': '"&amp;I37&amp;"', '"&amp;C$1&amp;"': "&amp;C37&amp;", '"&amp;D$1&amp;"': "&amp;D37&amp;", '"&amp;E$1&amp;"': '"&amp;E37&amp;"', '"&amp;F$1&amp;"': '"&amp;F37&amp;"', '"&amp;G$1&amp;"':"&amp;G37&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 99, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '1', 'offset':1}, </v>
       </c>
       <c r="K37" s="2" t="str">
-        <f>IF(B36=B37,CONCATENATE(K36,J37),J37)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 99, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '1', 'offset':1}, </v>
       </c>
       <c r="L37" s="11" t="str">
-        <f>IF(B37=B38,"","{'"&amp;B$1&amp;"': "&amp;B37&amp;", 'editing': false, 'tipo': '"&amp;A37&amp;"', 'data': "&amp;"["&amp;K37&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="174" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>159</v>
       </c>
@@ -3486,26 +3497,26 @@
         <v>172</v>
       </c>
       <c r="G38" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H38" s="14">
         <v>127</v>
       </c>
       <c r="J38" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H38&amp;", '"&amp;I$1&amp;"': '"&amp;I38&amp;"', '"&amp;C$1&amp;"': "&amp;C38&amp;", '"&amp;D$1&amp;"': "&amp;D38&amp;", '"&amp;E$1&amp;"': '"&amp;E38&amp;"', '"&amp;F$1&amp;"': '"&amp;F38&amp;"', '"&amp;G$1&amp;"':"&amp;G38&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 127, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'La contabilidad gerencial.\n‐ Qué es la contabilidad. El ciclo contable. Los Estados Financieros.\n‐Qué es la contabilidad gerencial. Objetivos e importancia de la contabilidad gerencial.\n‐Diferencias entre la contabilidad gerencial y la contabilidad financiera. Usuarios de la información. Tipo de información. Normas de regulación.', 'offset':1}, </v>
       </c>
       <c r="K38" s="2" t="str">
-        <f>IF(B37=B38,CONCATENATE(K37,J38),J38)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 99, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '1', 'offset':1}, { 'reg': 127, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'La contabilidad gerencial.\n‐ Qué es la contabilidad. El ciclo contable. Los Estados Financieros.\n‐Qué es la contabilidad gerencial. Objetivos e importancia de la contabilidad gerencial.\n‐Diferencias entre la contabilidad gerencial y la contabilidad financiera. Usuarios de la información. Tipo de información. Normas de regulación.', 'offset':1}, </v>
       </c>
       <c r="L38" s="11" t="str">
-        <f>IF(B38=B39,"","{'"&amp;B$1&amp;"': "&amp;B38&amp;", 'editing': false, 'tipo': '"&amp;A38&amp;"', 'data': "&amp;"["&amp;K38&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>159</v>
       </c>
@@ -3526,26 +3537,26 @@
         <v>68</v>
       </c>
       <c r="G39" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H39" s="14">
         <v>91</v>
       </c>
       <c r="J39" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H39&amp;", '"&amp;I$1&amp;"': '"&amp;I39&amp;"', '"&amp;C$1&amp;"': "&amp;C39&amp;", '"&amp;D$1&amp;"': "&amp;D39&amp;", '"&amp;E$1&amp;"': '"&amp;E39&amp;"', '"&amp;F$1&amp;"': '"&amp;F39&amp;"', '"&amp;G$1&amp;"':"&amp;G39&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 91, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Reconoce el recorrido de las operaciones empresariales en el ciclo contable de una empresa. Evalúa la utilidad de la información financiera y gerencial.', 'offset':1}, </v>
       </c>
       <c r="K39" s="2" t="str">
-        <f>IF(B38=B39,CONCATENATE(K38,J39),J39)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 99, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '1', 'offset':1}, { 'reg': 127, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'La contabilidad gerencial.\n‐ Qué es la contabilidad. El ciclo contable. Los Estados Financieros.\n‐Qué es la contabilidad gerencial. Objetivos e importancia de la contabilidad gerencial.\n‐Diferencias entre la contabilidad gerencial y la contabilidad financiera. Usuarios de la información. Tipo de información. Normas de regulación.', 'offset':1}, { 'reg': 91, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Reconoce el recorrido de las operaciones empresariales en el ciclo contable de una empresa. Evalúa la utilidad de la información financiera y gerencial.', 'offset':1}, </v>
       </c>
       <c r="L39" s="11" t="str">
-        <f>IF(B39=B40,"","{'"&amp;B$1&amp;"': "&amp;B39&amp;", 'editing': false, 'tipo': '"&amp;A39&amp;"', 'data': "&amp;"["&amp;K39&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>159</v>
       </c>
@@ -3566,26 +3577,26 @@
         <v>177</v>
       </c>
       <c r="G40" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H40" s="14">
         <v>115</v>
       </c>
       <c r="J40" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H40&amp;", '"&amp;I$1&amp;"': '"&amp;I40&amp;"', '"&amp;C$1&amp;"': "&amp;C40&amp;", '"&amp;D$1&amp;"': "&amp;D40&amp;", '"&amp;E$1&amp;"': '"&amp;E40&amp;"', '"&amp;F$1&amp;"': '"&amp;F40&amp;"', '"&amp;G$1&amp;"':"&amp;G40&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 115, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Exposición dialogada\nTaller', 'offset':1}, </v>
       </c>
       <c r="K40" s="2" t="str">
-        <f>IF(B39=B40,CONCATENATE(K39,J40),J40)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 99, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '1', 'offset':1}, { 'reg': 127, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'La contabilidad gerencial.\n‐ Qué es la contabilidad. El ciclo contable. Los Estados Financieros.\n‐Qué es la contabilidad gerencial. Objetivos e importancia de la contabilidad gerencial.\n‐Diferencias entre la contabilidad gerencial y la contabilidad financiera. Usuarios de la información. Tipo de información. Normas de regulación.', 'offset':1}, { 'reg': 91, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Reconoce el recorrido de las operaciones empresariales en el ciclo contable de una empresa. Evalúa la utilidad de la información financiera y gerencial.', 'offset':1}, { 'reg': 115, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Exposición dialogada\nTaller', 'offset':1}, </v>
       </c>
       <c r="L40" s="11" t="str">
-        <f>IF(B40=B41,"","{'"&amp;B$1&amp;"': "&amp;B40&amp;", 'editing': false, 'tipo': '"&amp;A40&amp;"', 'data': "&amp;"["&amp;K40&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 27, 'editing': false, 'tipo': 'contenidos', 'data': [{ 'reg': 99, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '1', 'offset':1}, { 'reg': 127, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'La contabilidad gerencial.\n‐ Qué es la contabilidad. El ciclo contable. Los Estados Financieros.\n‐Qué es la contabilidad gerencial. Objetivos e importancia de la contabilidad gerencial.\n‐Diferencias entre la contabilidad gerencial y la contabilidad financiera. Usuarios de la información. Tipo de información. Normas de regulación.', 'offset':1}, { 'reg': 91, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Reconoce el recorrido de las operaciones empresariales en el ciclo contable de una empresa. Evalúa la utilidad de la información financiera y gerencial.', 'offset':1}, { 'reg': 115, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Exposición dialogada\nTaller', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>159</v>
       </c>
@@ -3606,26 +3617,26 @@
         <v>2</v>
       </c>
       <c r="G41" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H41" s="14">
         <v>62</v>
       </c>
       <c r="J41" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H41&amp;", '"&amp;I$1&amp;"': '"&amp;I41&amp;"', '"&amp;C$1&amp;"': "&amp;C41&amp;", '"&amp;D$1&amp;"': "&amp;D41&amp;", '"&amp;E$1&amp;"': '"&amp;E41&amp;"', '"&amp;F$1&amp;"': '"&amp;F41&amp;"', '"&amp;G$1&amp;"':"&amp;G41&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '2', 'offset':1}, </v>
       </c>
       <c r="K41" s="2" t="str">
-        <f>IF(B40=B41,CONCATENATE(K40,J41),J41)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '2', 'offset':1}, </v>
       </c>
       <c r="L41" s="11" t="str">
-        <f>IF(B41=B42,"","{'"&amp;B$1&amp;"': "&amp;B41&amp;", 'editing': false, 'tipo': '"&amp;A41&amp;"', 'data': "&amp;"["&amp;K41&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>159</v>
       </c>
@@ -3646,26 +3657,26 @@
         <v>178</v>
       </c>
       <c r="G42" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H42" s="14">
         <v>17</v>
       </c>
       <c r="J42" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H42&amp;", '"&amp;I$1&amp;"': '"&amp;I42&amp;"', '"&amp;C$1&amp;"': "&amp;C42&amp;", '"&amp;D$1&amp;"': "&amp;D42&amp;", '"&amp;E$1&amp;"': '"&amp;E42&amp;"', '"&amp;F$1&amp;"': '"&amp;F42&amp;"', '"&amp;G$1&amp;"':"&amp;G42&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 17, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'La Contabilidad de Costos Empresariales.\n‐ Concepto. Importancia y su aplicación. Relación entre la contabilidad Gerencial y la Contabilidad de Costos.', 'offset':1}, </v>
       </c>
       <c r="K42" s="2" t="str">
-        <f>IF(B41=B42,CONCATENATE(K41,J42),J42)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '2', 'offset':1}, { 'reg': 17, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'La Contabilidad de Costos Empresariales.\n‐ Concepto. Importancia y su aplicación. Relación entre la contabilidad Gerencial y la Contabilidad de Costos.', 'offset':1}, </v>
       </c>
       <c r="L42" s="11" t="str">
-        <f>IF(B42=B43,"","{'"&amp;B$1&amp;"': "&amp;B42&amp;", 'editing': false, 'tipo': '"&amp;A42&amp;"', 'data': "&amp;"["&amp;K42&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="str">
         <f>+A42</f>
         <v>contenidos</v>
@@ -3687,26 +3698,26 @@
         <v>72</v>
       </c>
       <c r="G43" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H43" s="14">
         <v>102</v>
       </c>
       <c r="J43" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H43&amp;", '"&amp;I$1&amp;"': '"&amp;I43&amp;"', '"&amp;C$1&amp;"': "&amp;C43&amp;", '"&amp;D$1&amp;"': "&amp;D43&amp;", '"&amp;E$1&amp;"': '"&amp;E43&amp;"', '"&amp;F$1&amp;"': '"&amp;F43&amp;"', '"&amp;G$1&amp;"':"&amp;G43&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 102, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Determinación, distribución y aplicación de los costos en una empresa mercantil.', 'offset':1}, </v>
       </c>
       <c r="K43" s="2" t="str">
-        <f>IF(B42=B43,CONCATENATE(K42,J43),J43)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '2', 'offset':1}, { 'reg': 17, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'La Contabilidad de Costos Empresariales.\n‐ Concepto. Importancia y su aplicación. Relación entre la contabilidad Gerencial y la Contabilidad de Costos.', 'offset':1}, { 'reg': 102, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Determinación, distribución y aplicación de los costos en una empresa mercantil.', 'offset':1}, </v>
       </c>
       <c r="L43" s="11" t="str">
-        <f>IF(B43=B44,"","{'"&amp;B$1&amp;"': "&amp;B43&amp;", 'editing': false, 'tipo': '"&amp;A43&amp;"', 'data': "&amp;"["&amp;K43&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="str">
         <f>+A43</f>
         <v>contenidos</v>
@@ -3728,26 +3739,26 @@
         <v>73</v>
       </c>
       <c r="G44" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H44" s="14">
         <v>126</v>
       </c>
       <c r="J44" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H44&amp;", '"&amp;I$1&amp;"': '"&amp;I44&amp;"', '"&amp;C$1&amp;"': "&amp;C44&amp;", '"&amp;D$1&amp;"': "&amp;D44&amp;", '"&amp;E$1&amp;"': '"&amp;E44&amp;"', '"&amp;F$1&amp;"': '"&amp;F44&amp;"', '"&amp;G$1&amp;"':"&amp;G44&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 126, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Dinámica grupal/debate en clase', 'offset':1}, </v>
       </c>
       <c r="K44" s="2" t="str">
-        <f>IF(B43=B44,CONCATENATE(K43,J44),J44)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '2', 'offset':1}, { 'reg': 17, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'La Contabilidad de Costos Empresariales.\n‐ Concepto. Importancia y su aplicación. Relación entre la contabilidad Gerencial y la Contabilidad de Costos.', 'offset':1}, { 'reg': 102, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Determinación, distribución y aplicación de los costos en una empresa mercantil.', 'offset':1}, { 'reg': 126, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Dinámica grupal/debate en clase', 'offset':1}, </v>
       </c>
       <c r="L44" s="11" t="str">
-        <f>IF(B44=B45,"","{'"&amp;B$1&amp;"': "&amp;B44&amp;", 'editing': false, 'tipo': '"&amp;A44&amp;"', 'data': "&amp;"["&amp;K44&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 28, 'editing': false, 'tipo': 'contenidos', 'data': [{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '2', 'offset':1}, { 'reg': 17, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'La Contabilidad de Costos Empresariales.\n‐ Concepto. Importancia y su aplicación. Relación entre la contabilidad Gerencial y la Contabilidad de Costos.', 'offset':1}, { 'reg': 102, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Determinación, distribución y aplicación de los costos en una empresa mercantil.', 'offset':1}, { 'reg': 126, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Dinámica grupal/debate en clase', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>159</v>
       </c>
@@ -3768,26 +3779,26 @@
         <v>3</v>
       </c>
       <c r="G45" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H45" s="14">
         <v>39</v>
       </c>
       <c r="J45" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H45&amp;", '"&amp;I$1&amp;"': '"&amp;I45&amp;"', '"&amp;C$1&amp;"': "&amp;C45&amp;", '"&amp;D$1&amp;"': "&amp;D45&amp;", '"&amp;E$1&amp;"': '"&amp;E45&amp;"', '"&amp;F$1&amp;"': '"&amp;F45&amp;"', '"&amp;G$1&amp;"':"&amp;G45&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 39, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '3', 'offset':1}, </v>
       </c>
       <c r="K45" s="2" t="str">
-        <f>IF(B44=B45,CONCATENATE(K44,J45),J45)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 39, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '3', 'offset':1}, </v>
       </c>
       <c r="L45" s="11" t="str">
-        <f>IF(B45=B46,"","{'"&amp;B$1&amp;"': "&amp;B45&amp;", 'editing': false, 'tipo': '"&amp;A45&amp;"', 'data': "&amp;"["&amp;K45&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>159</v>
       </c>
@@ -3808,26 +3819,26 @@
         <v>173</v>
       </c>
       <c r="G46" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H46" s="14">
         <v>124</v>
       </c>
       <c r="J46" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H46&amp;", '"&amp;I$1&amp;"': '"&amp;I46&amp;"', '"&amp;C$1&amp;"': "&amp;C46&amp;", '"&amp;D$1&amp;"': "&amp;D46&amp;", '"&amp;E$1&amp;"': '"&amp;E46&amp;"', '"&amp;F$1&amp;"': '"&amp;F46&amp;"', '"&amp;G$1&amp;"':"&amp;G46&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 124, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'Elementos de los Estados Financieros:\n‐ Balance General: Activo, pasivo y patrimonio.\n‐ Estado de Resultados: Ingresos y Gastos', 'offset':1}, </v>
       </c>
       <c r="K46" s="2" t="str">
-        <f>IF(B45=B46,CONCATENATE(K45,J46),J46)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 39, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '3', 'offset':1}, { 'reg': 124, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'Elementos de los Estados Financieros:\n‐ Balance General: Activo, pasivo y patrimonio.\n‐ Estado de Resultados: Ingresos y Gastos', 'offset':1}, </v>
       </c>
       <c r="L46" s="11" t="str">
-        <f>IF(B46=B47,"","{'"&amp;B$1&amp;"': "&amp;B46&amp;", 'editing': false, 'tipo': '"&amp;A46&amp;"', 'data': "&amp;"["&amp;K46&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>159</v>
       </c>
@@ -3848,26 +3859,26 @@
         <v>77</v>
       </c>
       <c r="G47" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H47" s="14">
         <v>26</v>
       </c>
       <c r="J47" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H47&amp;", '"&amp;I$1&amp;"': '"&amp;I47&amp;"', '"&amp;C$1&amp;"': "&amp;C47&amp;", '"&amp;D$1&amp;"': "&amp;D47&amp;", '"&amp;E$1&amp;"': '"&amp;E47&amp;"', '"&amp;F$1&amp;"': '"&amp;F47&amp;"', '"&amp;G$1&amp;"':"&amp;G47&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 26, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Analizar y aplicar el marco legal normativo para la elaboración de los Estados Financieros.', 'offset':1}, </v>
       </c>
       <c r="K47" s="2" t="str">
-        <f>IF(B46=B47,CONCATENATE(K46,J47),J47)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 39, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '3', 'offset':1}, { 'reg': 124, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'Elementos de los Estados Financieros:\n‐ Balance General: Activo, pasivo y patrimonio.\n‐ Estado de Resultados: Ingresos y Gastos', 'offset':1}, { 'reg': 26, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Analizar y aplicar el marco legal normativo para la elaboración de los Estados Financieros.', 'offset':1}, </v>
       </c>
       <c r="L47" s="11" t="str">
-        <f>IF(B47=B48,"","{'"&amp;B$1&amp;"': "&amp;B47&amp;", 'editing': false, 'tipo': '"&amp;A47&amp;"', 'data': "&amp;"["&amp;K47&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>159</v>
       </c>
@@ -3888,26 +3899,26 @@
         <v>63</v>
       </c>
       <c r="G48" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H48" s="14">
         <v>40</v>
       </c>
       <c r="J48" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H48&amp;", '"&amp;I$1&amp;"': '"&amp;I48&amp;"', '"&amp;C$1&amp;"': "&amp;C48&amp;", '"&amp;D$1&amp;"': "&amp;D48&amp;", '"&amp;E$1&amp;"': '"&amp;E48&amp;"', '"&amp;F$1&amp;"': '"&amp;F48&amp;"', '"&amp;G$1&amp;"':"&amp;G48&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 40, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Exposición dialogada', 'offset':1}, </v>
       </c>
       <c r="K48" s="2" t="str">
-        <f>IF(B47=B48,CONCATENATE(K47,J48),J48)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 39, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '3', 'offset':1}, { 'reg': 124, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'Elementos de los Estados Financieros:\n‐ Balance General: Activo, pasivo y patrimonio.\n‐ Estado de Resultados: Ingresos y Gastos', 'offset':1}, { 'reg': 26, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Analizar y aplicar el marco legal normativo para la elaboración de los Estados Financieros.', 'offset':1}, { 'reg': 40, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Exposición dialogada', 'offset':1}, </v>
       </c>
       <c r="L48" s="11" t="str">
-        <f>IF(B48=B49,"","{'"&amp;B$1&amp;"': "&amp;B48&amp;", 'editing': false, 'tipo': '"&amp;A48&amp;"', 'data': "&amp;"["&amp;K48&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 29, 'editing': false, 'tipo': 'contenidos', 'data': [{ 'reg': 39, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '3', 'offset':1}, { 'reg': 124, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'Elementos de los Estados Financieros:\n‐ Balance General: Activo, pasivo y patrimonio.\n‐ Estado de Resultados: Ingresos y Gastos', 'offset':1}, { 'reg': 26, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Analizar y aplicar el marco legal normativo para la elaboración de los Estados Financieros.', 'offset':1}, { 'reg': 40, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Exposición dialogada', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>159</v>
       </c>
@@ -3928,26 +3939,26 @@
         <v>4</v>
       </c>
       <c r="G49" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H49" s="14">
         <v>43</v>
       </c>
       <c r="J49" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H49&amp;", '"&amp;I$1&amp;"': '"&amp;I49&amp;"', '"&amp;C$1&amp;"': "&amp;C49&amp;", '"&amp;D$1&amp;"': "&amp;D49&amp;", '"&amp;E$1&amp;"': '"&amp;E49&amp;"', '"&amp;F$1&amp;"': '"&amp;F49&amp;"', '"&amp;G$1&amp;"':"&amp;G49&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 43, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '4', 'offset':1}, </v>
       </c>
       <c r="K49" s="2" t="str">
-        <f>IF(B48=B49,CONCATENATE(K48,J49),J49)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 43, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '4', 'offset':1}, </v>
       </c>
       <c r="L49" s="11" t="str">
-        <f>IF(B49=B50,"","{'"&amp;B$1&amp;"': "&amp;B49&amp;", 'editing': false, 'tipo': '"&amp;A49&amp;"', 'data': "&amp;"["&amp;K49&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>159</v>
       </c>
@@ -3968,26 +3979,26 @@
         <v>174</v>
       </c>
       <c r="G50" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H50" s="14">
         <v>62</v>
       </c>
       <c r="J50" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H50&amp;", '"&amp;I$1&amp;"': '"&amp;I50&amp;"', '"&amp;C$1&amp;"': "&amp;C50&amp;", '"&amp;D$1&amp;"': "&amp;D50&amp;", '"&amp;E$1&amp;"': '"&amp;E50&amp;"', '"&amp;F$1&amp;"': '"&amp;F50&amp;"', '"&amp;G$1&amp;"':"&amp;G50&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'Análisis de los Estados Financieros\n‐Análisis Horizontal.\n‐Análisis Vertical.\n‐Desarrollo de casos de aplicación.\n‐ Elaboración de un informe gerencial.', 'offset':1}, </v>
       </c>
       <c r="K50" s="2" t="str">
-        <f>IF(B49=B50,CONCATENATE(K49,J50),J50)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 43, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '4', 'offset':1}, { 'reg': 62, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'Análisis de los Estados Financieros\n‐Análisis Horizontal.\n‐Análisis Vertical.\n‐Desarrollo de casos de aplicación.\n‐ Elaboración de un informe gerencial.', 'offset':1}, </v>
       </c>
       <c r="L50" s="11" t="str">
-        <f>IF(B50=B51,"","{'"&amp;B$1&amp;"': "&amp;B50&amp;", 'editing': false, 'tipo': '"&amp;A50&amp;"', 'data': "&amp;"["&amp;K50&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>159</v>
       </c>
@@ -4008,26 +4019,26 @@
         <v>85</v>
       </c>
       <c r="G51" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H51" s="14">
         <v>10</v>
       </c>
       <c r="J51" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H51&amp;", '"&amp;I$1&amp;"': '"&amp;I51&amp;"', '"&amp;C$1&amp;"': "&amp;C51&amp;", '"&amp;D$1&amp;"': "&amp;D51&amp;", '"&amp;E$1&amp;"': '"&amp;E51&amp;"', '"&amp;F$1&amp;"': '"&amp;F51&amp;"', '"&amp;G$1&amp;"':"&amp;G51&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 10, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Evalúa los resultados obtenidos. Demuestra la aplicación del análisis vertical y horizontal.', 'offset':1}, </v>
       </c>
       <c r="K51" s="2" t="str">
-        <f>IF(B50=B51,CONCATENATE(K50,J51),J51)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 43, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '4', 'offset':1}, { 'reg': 62, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'Análisis de los Estados Financieros\n‐Análisis Horizontal.\n‐Análisis Vertical.\n‐Desarrollo de casos de aplicación.\n‐ Elaboración de un informe gerencial.', 'offset':1}, { 'reg': 10, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Evalúa los resultados obtenidos. Demuestra la aplicación del análisis vertical y horizontal.', 'offset':1}, </v>
       </c>
       <c r="L51" s="11" t="str">
-        <f>IF(B51=B52,"","{'"&amp;B$1&amp;"': "&amp;B51&amp;", 'editing': false, 'tipo': '"&amp;A51&amp;"', 'data': "&amp;"["&amp;K51&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>159</v>
       </c>
@@ -4048,26 +4059,26 @@
         <v>175</v>
       </c>
       <c r="G52" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H52" s="14">
         <v>82</v>
       </c>
       <c r="J52" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H52&amp;", '"&amp;I$1&amp;"': '"&amp;I52&amp;"', '"&amp;C$1&amp;"': "&amp;C52&amp;", '"&amp;D$1&amp;"': "&amp;D52&amp;", '"&amp;E$1&amp;"': '"&amp;E52&amp;"', '"&amp;F$1&amp;"': '"&amp;F52&amp;"', '"&amp;G$1&amp;"':"&amp;G52&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 82, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Clase Expositiva\n Taller\n  Discusión de caso', 'offset':1}, </v>
       </c>
       <c r="K52" s="2" t="str">
-        <f>IF(B51=B52,CONCATENATE(K51,J52),J52)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 43, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '4', 'offset':1}, { 'reg': 62, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'Análisis de los Estados Financieros\n‐Análisis Horizontal.\n‐Análisis Vertical.\n‐Desarrollo de casos de aplicación.\n‐ Elaboración de un informe gerencial.', 'offset':1}, { 'reg': 10, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Evalúa los resultados obtenidos. Demuestra la aplicación del análisis vertical y horizontal.', 'offset':1}, { 'reg': 82, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Clase Expositiva\n Taller\n  Discusión de caso', 'offset':1}, </v>
       </c>
       <c r="L52" s="11" t="str">
-        <f>IF(B52=B53,"","{'"&amp;B$1&amp;"': "&amp;B52&amp;", 'editing': false, 'tipo': '"&amp;A52&amp;"', 'data': "&amp;"["&amp;K52&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 30, 'editing': false, 'tipo': 'contenidos', 'data': [{ 'reg': 43, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '4', 'offset':1}, { 'reg': 62, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'left', 'texto': 'Análisis de los Estados Financieros\n‐Análisis Horizontal.\n‐Análisis Vertical.\n‐Desarrollo de casos de aplicación.\n‐ Elaboración de un informe gerencial.', 'offset':1}, { 'reg': 10, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'left', 'texto': 'Evalúa los resultados obtenidos. Demuestra la aplicación del análisis vertical y horizontal.', 'offset':1}, { 'reg': 82, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'left', 'texto': 'Clase Expositiva\n Taller\n  Discusión de caso', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>161</v>
       </c>
@@ -4088,26 +4099,26 @@
         <v>160</v>
       </c>
       <c r="G53" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="H53" s="14">
         <v>19</v>
       </c>
       <c r="J53" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H53&amp;", '"&amp;I$1&amp;"': '"&amp;I53&amp;"', '"&amp;C$1&amp;"': "&amp;C53&amp;", '"&amp;D$1&amp;"': "&amp;D53&amp;", '"&amp;E$1&amp;"': '"&amp;E53&amp;"', '"&amp;F$1&amp;"': '"&amp;F53&amp;"', '"&amp;G$1&amp;"':"&amp;G53&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 19, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'center', 'texto': 'EVALUACIÓN PARCIAL 1 ', 'offset':2}, </v>
       </c>
       <c r="K53" s="2" t="str">
-        <f>IF(B52=B53,CONCATENATE(K52,J53),J53)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 19, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'center', 'texto': 'EVALUACIÓN PARCIAL 1 ', 'offset':2}, </v>
       </c>
       <c r="L53" s="11" t="str">
-        <f>IF(B53=B54,"","{'"&amp;B$1&amp;"': "&amp;B53&amp;", 'editing': false, 'tipo': '"&amp;A53&amp;"', 'data': "&amp;"["&amp;K53&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 31, 'editing': false, 'tipo': 'evaluaciones', 'data': [{ 'reg': 19, 'subtipo': '', 'col': 2, 'cols': 7, 'align': 'center', 'texto': 'EVALUACIÓN PARCIAL 1 ', 'offset':2}, ],  },</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>159</v>
       </c>
@@ -4128,26 +4139,26 @@
         <v>5</v>
       </c>
       <c r="G54" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H54" s="14">
         <v>82</v>
       </c>
       <c r="J54" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H54&amp;", '"&amp;I$1&amp;"': '"&amp;I54&amp;"', '"&amp;C$1&amp;"': "&amp;C54&amp;", '"&amp;D$1&amp;"': "&amp;D54&amp;", '"&amp;E$1&amp;"': '"&amp;E54&amp;"', '"&amp;F$1&amp;"': '"&amp;F54&amp;"', '"&amp;G$1&amp;"':"&amp;G54&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 82, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '5', 'offset':1}, </v>
       </c>
       <c r="K54" s="2" t="str">
-        <f>IF(B53=B54,CONCATENATE(K53,J54),J54)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 82, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '5', 'offset':1}, </v>
       </c>
       <c r="L54" s="11" t="str">
-        <f>IF(B54=B55,"","{'"&amp;B$1&amp;"': "&amp;B54&amp;", 'editing': false, 'tipo': '"&amp;A54&amp;"', 'data': "&amp;"["&amp;K54&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>159</v>
       </c>
@@ -4165,26 +4176,26 @@
         <v>176</v>
       </c>
       <c r="G55" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H55" s="14">
         <v>61</v>
       </c>
       <c r="J55" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H55&amp;", '"&amp;I$1&amp;"': '"&amp;I55&amp;"', '"&amp;C$1&amp;"': "&amp;C55&amp;", '"&amp;D$1&amp;"': "&amp;D55&amp;", '"&amp;E$1&amp;"': '"&amp;E55&amp;"', '"&amp;F$1&amp;"': '"&amp;F55&amp;"', '"&amp;G$1&amp;"':"&amp;G55&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 61, 'subtipo': '', 'col': 2, 'cols': 3, 'align': '', 'texto': 'Trabajos de aplicación\n ‐Análisis de todo el proceso aplicado hasta el informe gerencial.', 'offset':1}, </v>
       </c>
       <c r="K55" s="2" t="str">
-        <f>IF(B54=B55,CONCATENATE(K54,J55),J55)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 82, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '5', 'offset':1}, { 'reg': 61, 'subtipo': '', 'col': 2, 'cols': 3, 'align': '', 'texto': 'Trabajos de aplicación\n ‐Análisis de todo el proceso aplicado hasta el informe gerencial.', 'offset':1}, </v>
       </c>
       <c r="L55" s="11" t="str">
-        <f>IF(B55=B56,"","{'"&amp;B$1&amp;"': "&amp;B55&amp;", 'editing': false, 'tipo': '"&amp;A55&amp;"', 'data': "&amp;"["&amp;K55&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>159</v>
       </c>
@@ -4202,26 +4213,26 @@
         <v>89</v>
       </c>
       <c r="G56" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H56" s="14">
         <v>39</v>
       </c>
       <c r="J56" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H56&amp;", '"&amp;I$1&amp;"': '"&amp;I56&amp;"', '"&amp;C$1&amp;"': "&amp;C56&amp;", '"&amp;D$1&amp;"': "&amp;D56&amp;", '"&amp;E$1&amp;"': '"&amp;E56&amp;"', '"&amp;F$1&amp;"': '"&amp;F56&amp;"', '"&amp;G$1&amp;"':"&amp;G56&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 39, 'subtipo': '', 'col': 4, 'cols': 2, 'align': '', 'texto': 'Propicia un debate acerca de la toma de decisiones en una empresa.', 'offset':1}, </v>
       </c>
       <c r="K56" s="2" t="str">
-        <f>IF(B55=B56,CONCATENATE(K55,J56),J56)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 82, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '5', 'offset':1}, { 'reg': 61, 'subtipo': '', 'col': 2, 'cols': 3, 'align': '', 'texto': 'Trabajos de aplicación\n ‐Análisis de todo el proceso aplicado hasta el informe gerencial.', 'offset':1}, { 'reg': 39, 'subtipo': '', 'col': 4, 'cols': 2, 'align': '', 'texto': 'Propicia un debate acerca de la toma de decisiones en una empresa.', 'offset':1}, </v>
       </c>
       <c r="L56" s="11" t="str">
-        <f>IF(B56=B57,"","{'"&amp;B$1&amp;"': "&amp;B56&amp;", 'editing': false, 'tipo': '"&amp;A56&amp;"', 'data': "&amp;"["&amp;K56&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>159</v>
       </c>
@@ -4239,26 +4250,26 @@
         <v>63</v>
       </c>
       <c r="G57" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H57" s="14">
         <v>69</v>
       </c>
       <c r="J57" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H57&amp;", '"&amp;I$1&amp;"': '"&amp;I57&amp;"', '"&amp;C$1&amp;"': "&amp;C57&amp;", '"&amp;D$1&amp;"': "&amp;D57&amp;", '"&amp;E$1&amp;"': '"&amp;E57&amp;"', '"&amp;F$1&amp;"': '"&amp;F57&amp;"', '"&amp;G$1&amp;"':"&amp;G57&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 69, 'subtipo': '', 'col': 6, 'cols': 2, 'align': '', 'texto': 'Exposición dialogada', 'offset':1}, </v>
       </c>
       <c r="K57" s="2" t="str">
-        <f>IF(B56=B57,CONCATENATE(K56,J57),J57)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 82, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '5', 'offset':1}, { 'reg': 61, 'subtipo': '', 'col': 2, 'cols': 3, 'align': '', 'texto': 'Trabajos de aplicación\n ‐Análisis de todo el proceso aplicado hasta el informe gerencial.', 'offset':1}, { 'reg': 39, 'subtipo': '', 'col': 4, 'cols': 2, 'align': '', 'texto': 'Propicia un debate acerca de la toma de decisiones en una empresa.', 'offset':1}, { 'reg': 69, 'subtipo': '', 'col': 6, 'cols': 2, 'align': '', 'texto': 'Exposición dialogada', 'offset':1}, </v>
       </c>
       <c r="L57" s="11" t="str">
-        <f>IF(B57=B58,"","{'"&amp;B$1&amp;"': "&amp;B57&amp;", 'editing': false, 'tipo': '"&amp;A57&amp;"', 'data': "&amp;"["&amp;K57&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 32, 'editing': false, 'tipo': 'contenidos', 'data': [{ 'reg': 82, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': '5', 'offset':1}, { 'reg': 61, 'subtipo': '', 'col': 2, 'cols': 3, 'align': '', 'texto': 'Trabajos de aplicación\n ‐Análisis de todo el proceso aplicado hasta el informe gerencial.', 'offset':1}, { 'reg': 39, 'subtipo': '', 'col': 4, 'cols': 2, 'align': '', 'texto': 'Propicia un debate acerca de la toma de decisiones en una empresa.', 'offset':1}, { 'reg': 69, 'subtipo': '', 'col': 6, 'cols': 2, 'align': '', 'texto': 'Exposición dialogada', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>158</v>
       </c>
@@ -4279,26 +4290,26 @@
         <v>170</v>
       </c>
       <c r="G58" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H58" s="14">
         <v>124</v>
       </c>
       <c r="J58" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H58&amp;", '"&amp;I$1&amp;"': '"&amp;I58&amp;"', '"&amp;C$1&amp;"': "&amp;C58&amp;", '"&amp;D$1&amp;"': "&amp;D58&amp;", '"&amp;E$1&amp;"': '"&amp;E58&amp;"', '"&amp;F$1&amp;"': '"&amp;F58&amp;"', '"&amp;G$1&amp;"':"&amp;G58&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 124, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'center', 'texto': 'UNIDAD II: ANALISIS E INTERPRETACION DE LOS ESTADOS FINANCIEROS', 'offset':1}, </v>
       </c>
       <c r="K58" s="2" t="str">
-        <f>IF(B57=B58,CONCATENATE(K57,J58),J58)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 124, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'center', 'texto': 'UNIDAD II: ANALISIS E INTERPRETACION DE LOS ESTADOS FINANCIEROS', 'offset':1}, </v>
       </c>
       <c r="L58" s="11" t="str">
-        <f>IF(B58=B59,"","{'"&amp;B$1&amp;"': "&amp;B58&amp;", 'editing': false, 'tipo': '"&amp;A58&amp;"', 'data': "&amp;"["&amp;K58&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 33, 'editing': false, 'tipo': 'unidades', 'data': [{ 'reg': 124, 'subtipo': '', 'col': 1, 'cols': 8, 'align': 'center', 'texto': 'UNIDAD II: ANALISIS E INTERPRETACION DE LOS ESTADOS FINANCIEROS', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>157</v>
       </c>
@@ -4319,26 +4330,26 @@
         <v>59</v>
       </c>
       <c r="G59" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H59" s="14">
         <v>62</v>
       </c>
       <c r="J59" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H59&amp;", '"&amp;I$1&amp;"': '"&amp;I59&amp;"', '"&amp;C$1&amp;"': "&amp;C59&amp;", '"&amp;D$1&amp;"': "&amp;D59&amp;", '"&amp;E$1&amp;"': '"&amp;E59&amp;"', '"&amp;F$1&amp;"': '"&amp;F59&amp;"', '"&amp;G$1&amp;"':"&amp;G59&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, </v>
       </c>
       <c r="K59" s="2" t="str">
-        <f>IF(B58=B59,CONCATENATE(K58,J59),J59)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, </v>
       </c>
       <c r="L59" s="11" t="str">
-        <f>IF(B59=B60,"","{'"&amp;B$1&amp;"': "&amp;B59&amp;", 'editing': false, 'tipo': '"&amp;A59&amp;"', 'data': "&amp;"["&amp;K59&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>157</v>
       </c>
@@ -4359,26 +4370,26 @@
         <v>60</v>
       </c>
       <c r="G60" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H60" s="14">
         <v>61</v>
       </c>
       <c r="J60" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H60&amp;", '"&amp;I$1&amp;"': '"&amp;I60&amp;"', '"&amp;C$1&amp;"': "&amp;C60&amp;", '"&amp;D$1&amp;"': "&amp;D60&amp;", '"&amp;E$1&amp;"': '"&amp;E60&amp;"', '"&amp;F$1&amp;"': '"&amp;F60&amp;"', '"&amp;G$1&amp;"':"&amp;G60&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 61, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'center', 'texto': 'CONCEPTUAL', 'offset':1}, </v>
       </c>
       <c r="K60" s="2" t="str">
-        <f>IF(B59=B60,CONCATENATE(K59,J60),J60)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, { 'reg': 61, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'center', 'texto': 'CONCEPTUAL', 'offset':1}, </v>
       </c>
       <c r="L60" s="11" t="str">
-        <f>IF(B60=B61,"","{'"&amp;B$1&amp;"': "&amp;B60&amp;", 'editing': false, 'tipo': '"&amp;A60&amp;"', 'data': "&amp;"["&amp;K60&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>157</v>
       </c>
@@ -4399,26 +4410,26 @@
         <v>61</v>
       </c>
       <c r="G61" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H61" s="14">
         <v>73</v>
       </c>
       <c r="J61" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H61&amp;", '"&amp;I$1&amp;"': '"&amp;I61&amp;"', '"&amp;C$1&amp;"': "&amp;C61&amp;", '"&amp;D$1&amp;"': "&amp;D61&amp;", '"&amp;E$1&amp;"': '"&amp;E61&amp;"', '"&amp;F$1&amp;"': '"&amp;F61&amp;"', '"&amp;G$1&amp;"':"&amp;G61&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 73, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'center', 'texto': 'PROCEDIMENTAL', 'offset':1}, </v>
       </c>
       <c r="K61" s="2" t="str">
-        <f>IF(B60=B61,CONCATENATE(K60,J61),J61)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, { 'reg': 61, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'center', 'texto': 'CONCEPTUAL', 'offset':1}, { 'reg': 73, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'center', 'texto': 'PROCEDIMENTAL', 'offset':1}, </v>
       </c>
       <c r="L61" s="11" t="str">
-        <f>IF(B61=B62,"","{'"&amp;B$1&amp;"': "&amp;B61&amp;", 'editing': false, 'tipo': '"&amp;A61&amp;"', 'data': "&amp;"["&amp;K61&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>157</v>
       </c>
@@ -4439,26 +4450,26 @@
         <v>62</v>
       </c>
       <c r="G62" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H62" s="14">
         <v>27</v>
       </c>
       <c r="J62" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H62&amp;", '"&amp;I$1&amp;"': '"&amp;I62&amp;"', '"&amp;C$1&amp;"': "&amp;C62&amp;", '"&amp;D$1&amp;"': "&amp;D62&amp;", '"&amp;E$1&amp;"': '"&amp;E62&amp;"', '"&amp;F$1&amp;"': '"&amp;F62&amp;"', '"&amp;G$1&amp;"':"&amp;G62&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 27, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'center', 'texto': 'ACTIVIDAD DE APRENDIZAJE', 'offset':1}, </v>
       </c>
       <c r="K62" s="2" t="str">
-        <f>IF(B61=B62,CONCATENATE(K61,J62),J62)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, { 'reg': 61, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'center', 'texto': 'CONCEPTUAL', 'offset':1}, { 'reg': 73, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'center', 'texto': 'PROCEDIMENTAL', 'offset':1}, { 'reg': 27, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'center', 'texto': 'ACTIVIDAD DE APRENDIZAJE', 'offset':1}, </v>
       </c>
       <c r="L62" s="11" t="str">
-        <f>IF(B62=B63,"","{'"&amp;B$1&amp;"': "&amp;B62&amp;", 'editing': false, 'tipo': '"&amp;A62&amp;"', 'data': "&amp;"["&amp;K62&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 34, 'editing': false, 'tipo': 'titulo3', 'data': [{ 'reg': 62, 'subtipo': '', 'col': 1, 'cols': 1, 'align': 'center', 'texto': 'SEMANA', 'offset':1}, { 'reg': 61, 'subtipo': '', 'col': 2, 'cols': 3, 'align': 'center', 'texto': 'CONCEPTUAL', 'offset':1}, { 'reg': 73, 'subtipo': '', 'col': 4, 'cols': 2, 'align': 'center', 'texto': 'PROCEDIMENTAL', 'offset':1}, { 'reg': 27, 'subtipo': '', 'col': 6, 'cols': 2, 'align': 'center', 'texto': 'ACTIVIDAD DE APRENDIZAJE', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>151</v>
       </c>
@@ -4479,7 +4490,7 @@
         <v>166</v>
       </c>
       <c r="G63" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H63" s="14">
@@ -4489,24 +4500,24 @@
         <v>181</v>
       </c>
       <c r="J63" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H63&amp;", '"&amp;I$1&amp;"': '"&amp;I63&amp;"', '"&amp;C$1&amp;"': "&amp;C63&amp;", '"&amp;D$1&amp;"': "&amp;D63&amp;", '"&amp;E$1&amp;"': '"&amp;E63&amp;"', '"&amp;F$1&amp;"': '"&amp;F63&amp;"', '"&amp;G$1&amp;"':"&amp;G63&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 6, 'subtipo': 'estrategias', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'V. ESTRATEGIAS METODOLÓGICAS', 'offset':1}, </v>
       </c>
       <c r="K63" s="2" t="str">
-        <f>IF(B62=B63,CONCATENATE(K62,J63),J63)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 6, 'subtipo': 'estrategias', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'V. ESTRATEGIAS METODOLÓGICAS', 'offset':1}, </v>
       </c>
       <c r="L63" s="11" t="str">
-        <f>IF(B63=B64,"","{'"&amp;B$1&amp;"': "&amp;B63&amp;", 'editing': false, 'tipo': '"&amp;A63&amp;"', 'data': "&amp;"["&amp;K63&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 35, 'editing': false, 'tipo': 'titulo1', 'data': [{ 'reg': 6, 'subtipo': 'estrategias', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'V. ESTRATEGIAS METODOLÓGICAS', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B64" s="2">
-        <f t="shared" ref="B64:B65" si="3">+B63+1</f>
+        <f t="shared" ref="B64:B65" si="9">+B63+1</f>
         <v>36</v>
       </c>
       <c r="C64" s="2">
@@ -4522,7 +4533,7 @@
         <v>167</v>
       </c>
       <c r="G64" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H64" s="14">
@@ -4532,24 +4543,24 @@
         <v>161</v>
       </c>
       <c r="J64" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H64&amp;", '"&amp;I$1&amp;"': '"&amp;I64&amp;"', '"&amp;C$1&amp;"': "&amp;C64&amp;", '"&amp;D$1&amp;"': "&amp;D64&amp;", '"&amp;E$1&amp;"': '"&amp;E64&amp;"', '"&amp;F$1&amp;"': '"&amp;F64&amp;"', '"&amp;G$1&amp;"':"&amp;G64&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 75, 'subtipo': 'evaluaciones', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'VI. EVALUACIÓN', 'offset':1}, </v>
       </c>
       <c r="K64" s="2" t="str">
-        <f>IF(B63=B64,CONCATENATE(K63,J64),J64)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 75, 'subtipo': 'evaluaciones', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'VI. EVALUACIÓN', 'offset':1}, </v>
       </c>
       <c r="L64" s="11" t="str">
-        <f>IF(B64=B65,"","{'"&amp;B$1&amp;"': "&amp;B64&amp;", 'editing': false, 'tipo': '"&amp;A64&amp;"', 'data': "&amp;"["&amp;K64&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 36, 'editing': false, 'tipo': 'titulo1', 'data': [{ 'reg': 75, 'subtipo': 'evaluaciones', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'VI. EVALUACIÓN', 'offset':1}, ],  },</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B65" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>37</v>
       </c>
       <c r="C65" s="2">
@@ -4565,7 +4576,7 @@
         <v>168</v>
       </c>
       <c r="G65" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H65" s="14">
@@ -4575,17 +4586,29 @@
         <v>182</v>
       </c>
       <c r="J65" s="15" t="str">
-        <f>+"{ '"&amp;H$1&amp;"': "&amp;H65&amp;", '"&amp;I$1&amp;"': '"&amp;I65&amp;"', '"&amp;C$1&amp;"': "&amp;C65&amp;", '"&amp;D$1&amp;"': "&amp;D65&amp;", '"&amp;E$1&amp;"': '"&amp;E65&amp;"', '"&amp;F$1&amp;"': '"&amp;F65&amp;"', '"&amp;G$1&amp;"':"&amp;G65&amp;"}, "</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">{ 'reg': 102, 'subtipo': 'bibliografias', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'VII. BIBLIOGRAFÍA', 'offset':1}, </v>
       </c>
       <c r="K65" s="2" t="str">
-        <f>IF(B64=B65,CONCATENATE(K64,J65),J65)</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">{ 'reg': 102, 'subtipo': 'bibliografias', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'VII. BIBLIOGRAFÍA', 'offset':1}, </v>
       </c>
       <c r="L65" s="11" t="str">
-        <f>IF(B65=B66,"","{'"&amp;B$1&amp;"': "&amp;B65&amp;", 'editing': false, 'tipo': '"&amp;A65&amp;"', 'data': "&amp;"["&amp;K65&amp;"],  },")</f>
+        <f t="shared" si="8"/>
         <v>{'row': 37, 'editing': false, 'tipo': 'titulo1', 'data': [{ 'reg': 102, 'subtipo': 'bibliografias', 'col': 1, 'cols': 8, 'align': 'left', 'texto': 'VII. BIBLIOGRAFÍA', 'offset':1}, ],  },</v>
       </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F70" s="16"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F71" s="16"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F72" s="16"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F73" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F65"/>
@@ -4603,18 +4626,18 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>134</v>
       </c>
@@ -4631,7 +4654,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Delete Sumillas and Contenidos only phpunit
</commit_message>
<xml_diff>
--- a/topdown.xlsx
+++ b/topdown.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="265">
   <si>
     <t xml:space="preserve">Componente</t>
   </si>
@@ -796,28 +796,31 @@
     <t xml:space="preserve">'contenido’</t>
   </si>
   <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Nuevo registro’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Editar’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click Nuevo registro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">textArea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Grabar’</t>
+  </si>
+  <si>
     <t xml:space="preserve">hidden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'Nuevo registro’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">view</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'Editar’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click Nuevo registro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new</t>
-  </si>
-  <si>
-    <t xml:space="preserve">textArea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'Grabar’</t>
   </si>
   <si>
     <t xml:space="preserve">Click Grabar (registro new)</t>
@@ -5332,10 +5335,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ9"/>
+  <dimension ref="A1:AMJ10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5412,6 +5415,12 @@
       <c r="B4" s="8" t="s">
         <v>252</v>
       </c>
+      <c r="C4" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0</v>
+      </c>
       <c r="E4" s="24" t="s">
         <v>253</v>
       </c>
@@ -5442,15 +5451,15 @@
         <v>260</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>249</v>
@@ -5459,7 +5468,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>254</v>
@@ -5472,32 +5481,23 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>262</v>
-      </c>
       <c r="C8" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D8" s="8" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="E8" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="F8" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="J8" s="25" t="s">
+      <c r="F8" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="K8" s="25" t="s">
-        <v>253</v>
+      <c r="K8" s="8" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5505,21 +5505,50 @@
         <v>263</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D9" s="8" t="n">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="E9" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K10" s="8" t="s">
         <v>256</v>
       </c>
     </row>

</xml_diff>